<commit_message>
Updated  status columnb in excel file
</commit_message>
<xml_diff>
--- a/IT23242104_FIXED.xlsx
+++ b/IT23242104_FIXED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sliit\IT23242104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08922394-E605-4BF9-9777-4B61BA3C8060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CD025B-3771-45E3-A556-EE15F5F4D183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4164" yWindow="1296" windowWidth="17280" windowHeight="10608" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="269">
   <si>
     <t>TC ID</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t xml:space="preserve">  Copy-Paste behavior</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -962,8 +965,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -973,14 +976,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1324,7 +1327,7 @@
   <dimension ref="B2:J221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D141" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="H165" sqref="H165"/>
+      <selection activeCell="H157" sqref="H157:H160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,26 +1337,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="14"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1385,7 +1388,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -1414,42 +1417,42 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1478,13 +1481,13 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1493,13 +1496,13 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1508,18 +1511,18 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -1548,13 +1551,13 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="5" t="s">
         <v>35</v>
       </c>
@@ -1563,27 +1566,27 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
       <c r="J16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1618,38 +1621,38 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="2:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1684,13 +1687,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1699,13 +1702,13 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="9" t="s">
         <v>54</v>
       </c>
@@ -1714,15 +1717,15 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
@@ -1754,13 +1757,13 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="9" t="s">
         <v>54</v>
       </c>
@@ -1769,28 +1772,28 @@
       </c>
     </row>
     <row r="27" spans="2:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
       <c r="J27" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
     </row>
     <row r="29" spans="2:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
@@ -1822,40 +1825,40 @@
       </c>
     </row>
     <row r="30" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
       <c r="J30" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
       <c r="J32" s="2" t="s">
         <v>69</v>
       </c>
@@ -1890,40 +1893,40 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
       <c r="J34" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
       <c r="J35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
       <c r="J36" s="2" t="s">
         <v>17</v>
       </c>
@@ -1958,41 +1961,41 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
       <c r="J38" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
       <c r="J39" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
     </row>
     <row r="41" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
@@ -2024,41 +2027,41 @@
       </c>
     </row>
     <row r="42" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
       <c r="J42" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
       <c r="J43" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
     </row>
     <row r="45" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
@@ -2090,39 +2093,39 @@
       </c>
     </row>
     <row r="46" spans="2:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="7"/>
     </row>
     <row r="47" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
       <c r="J47" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
     </row>
     <row r="49" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
@@ -2154,39 +2157,39 @@
       </c>
     </row>
     <row r="50" spans="2:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="7"/>
     </row>
     <row r="51" spans="2:10" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
       <c r="J51" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
     </row>
     <row r="53" spans="2:10" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="5" t="s">
@@ -2218,13 +2221,13 @@
       </c>
     </row>
     <row r="54" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
       <c r="I54" s="9" t="s">
         <v>25</v>
       </c>
@@ -2233,24 +2236,24 @@
       </c>
     </row>
     <row r="55" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
     </row>
     <row r="56" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
       <c r="I56" s="4" t="s">
         <v>111</v>
       </c>
@@ -2288,41 +2291,41 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
       <c r="J58" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
       <c r="J59" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
     </row>
     <row r="61" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="5" t="s">
@@ -2354,39 +2357,39 @@
       </c>
     </row>
     <row r="62" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="7"/>
     </row>
     <row r="63" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
       <c r="J63" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
     </row>
     <row r="65" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
@@ -2418,41 +2421,41 @@
       </c>
     </row>
     <row r="66" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
       <c r="J66" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="67" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
       <c r="J67" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="68" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
     </row>
     <row r="69" spans="2:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="5" t="s">
@@ -2484,38 +2487,38 @@
       </c>
     </row>
     <row r="70" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
       <c r="J70" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="7"/>
     </row>
     <row r="72" spans="2:10" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
       <c r="J72" s="2" t="s">
         <v>134</v>
       </c>
@@ -2550,38 +2553,38 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
       <c r="J74" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="7"/>
     </row>
     <row r="76" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
       <c r="J76" s="2" t="s">
         <v>77</v>
       </c>
@@ -2616,41 +2619,41 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="7"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
       <c r="J78" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
       <c r="J79" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="80" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
     </row>
     <row r="81" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="5" t="s">
@@ -2682,41 +2685,41 @@
       </c>
     </row>
     <row r="82" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
       <c r="J82" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="83" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
-      <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="7"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
       <c r="J83" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="84" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="7"/>
     </row>
     <row r="85" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="5" t="s">
@@ -2748,13 +2751,13 @@
       </c>
     </row>
     <row r="86" spans="2:10" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
       <c r="I86" s="9" t="s">
         <v>161</v>
       </c>
@@ -2763,27 +2766,27 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="I87" s="7"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
       <c r="J87" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="88" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
-      <c r="H88" s="6"/>
-      <c r="I88" s="6"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
       <c r="J88" s="2" t="s">
         <v>77</v>
       </c>
@@ -2818,41 +2821,41 @@
       </c>
     </row>
     <row r="90" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
-      <c r="I90" s="7"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
       <c r="J90" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="7"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
       <c r="J91" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="6"/>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="6"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+      <c r="I92" s="7"/>
+      <c r="J92" s="7"/>
     </row>
     <row r="93" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
@@ -2884,41 +2887,41 @@
       </c>
     </row>
     <row r="94" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="7"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="I94" s="7"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
       <c r="J94" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="95" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="7"/>
-      <c r="E95" s="7"/>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="7"/>
-      <c r="I95" s="7"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
       <c r="J95" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="96" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="6"/>
-      <c r="J96" s="6"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
+      <c r="I96" s="7"/>
+      <c r="J96" s="7"/>
     </row>
     <row r="97" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="5" t="s">
@@ -2950,41 +2953,41 @@
       </c>
     </row>
     <row r="98" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
       <c r="J98" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="99" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
       <c r="J99" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="100" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="6"/>
-      <c r="H100" s="6"/>
-      <c r="I100" s="6"/>
-      <c r="J100" s="6"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+      <c r="J100" s="7"/>
     </row>
     <row r="101" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
@@ -3016,41 +3019,41 @@
       </c>
     </row>
     <row r="102" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
       <c r="J102" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="103" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
-      <c r="H103" s="7"/>
-      <c r="I103" s="7"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
       <c r="J103" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="104" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="6"/>
-      <c r="J104" s="6"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
     </row>
     <row r="105" spans="2:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="5" t="s">
@@ -3082,39 +3085,39 @@
       </c>
     </row>
     <row r="106" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
-      <c r="J106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="7"/>
     </row>
     <row r="107" spans="2:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
       <c r="J107" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="108" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="6"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
-      <c r="I108" s="6"/>
-      <c r="J108" s="6"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
     </row>
     <row r="109" spans="2:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="5" t="s">
@@ -3146,39 +3149,39 @@
       </c>
     </row>
     <row r="110" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
-      <c r="I110" s="7"/>
-      <c r="J110" s="6"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="7"/>
     </row>
     <row r="111" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7"/>
-      <c r="F111" s="7"/>
-      <c r="G111" s="7"/>
-      <c r="H111" s="7"/>
-      <c r="I111" s="7"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
       <c r="J111" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="112" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
-      <c r="F112" s="6"/>
-      <c r="G112" s="6"/>
-      <c r="H112" s="6"/>
-      <c r="I112" s="6"/>
-      <c r="J112" s="6"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
     </row>
     <row r="113" spans="2:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="5" t="s">
@@ -3210,39 +3213,39 @@
       </c>
     </row>
     <row r="114" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7"/>
-      <c r="F114" s="7"/>
-      <c r="G114" s="7"/>
-      <c r="H114" s="7"/>
-      <c r="I114" s="7"/>
-      <c r="J114" s="6"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="7"/>
     </row>
     <row r="115" spans="2:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7"/>
-      <c r="G115" s="7"/>
-      <c r="H115" s="7"/>
-      <c r="I115" s="7"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
       <c r="J115" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="116" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="6"/>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
-      <c r="G116" s="6"/>
-      <c r="H116" s="6"/>
-      <c r="I116" s="6"/>
-      <c r="J116" s="6"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
     </row>
     <row r="117" spans="2:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="5" t="s">
@@ -3274,39 +3277,39 @@
       </c>
     </row>
     <row r="118" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
-      <c r="D118" s="7"/>
-      <c r="E118" s="7"/>
-      <c r="F118" s="7"/>
-      <c r="G118" s="7"/>
-      <c r="H118" s="7"/>
-      <c r="I118" s="7"/>
-      <c r="J118" s="6"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="7"/>
     </row>
     <row r="119" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="I119" s="7"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
       <c r="J119" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="120" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
-      <c r="I120" s="6"/>
-      <c r="J120" s="6"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
+      <c r="G120" s="7"/>
+      <c r="H120" s="7"/>
+      <c r="I120" s="7"/>
+      <c r="J120" s="7"/>
     </row>
     <row r="121" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="5" t="s">
@@ -3338,39 +3341,39 @@
       </c>
     </row>
     <row r="122" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
-      <c r="G122" s="7"/>
-      <c r="H122" s="7"/>
-      <c r="I122" s="7"/>
-      <c r="J122" s="6"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+      <c r="I122" s="6"/>
+      <c r="J122" s="7"/>
     </row>
     <row r="123" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
-      <c r="D123" s="7"/>
-      <c r="E123" s="7"/>
-      <c r="F123" s="7"/>
-      <c r="G123" s="7"/>
-      <c r="H123" s="7"/>
-      <c r="I123" s="7"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
       <c r="J123" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="124" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="6"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="6"/>
-      <c r="G124" s="6"/>
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
-      <c r="J124" s="6"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
+      <c r="G124" s="7"/>
+      <c r="H124" s="7"/>
+      <c r="I124" s="7"/>
+      <c r="J124" s="7"/>
     </row>
     <row r="125" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="5" t="s">
@@ -3402,39 +3405,39 @@
       </c>
     </row>
     <row r="126" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="7"/>
-      <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
-      <c r="G126" s="7"/>
-      <c r="H126" s="7"/>
-      <c r="I126" s="7"/>
-      <c r="J126" s="6"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="7"/>
     </row>
     <row r="127" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="7"/>
-      <c r="I127" s="7"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
       <c r="J127" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="128" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="6"/>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="6"/>
-      <c r="G128" s="6"/>
-      <c r="H128" s="6"/>
-      <c r="I128" s="6"/>
-      <c r="J128" s="6"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
+      <c r="E128" s="7"/>
+      <c r="F128" s="7"/>
+      <c r="G128" s="7"/>
+      <c r="H128" s="7"/>
+      <c r="I128" s="7"/>
+      <c r="J128" s="7"/>
     </row>
     <row r="129" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="5" t="s">
@@ -3466,39 +3469,39 @@
       </c>
     </row>
     <row r="130" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="7"/>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7"/>
-      <c r="E130" s="7"/>
-      <c r="F130" s="7"/>
-      <c r="G130" s="7"/>
-      <c r="H130" s="7"/>
-      <c r="I130" s="7"/>
-      <c r="J130" s="6"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="6"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="7"/>
     </row>
     <row r="131" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
-      <c r="F131" s="7"/>
-      <c r="G131" s="7"/>
-      <c r="H131" s="7"/>
-      <c r="I131" s="7"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
       <c r="J131" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="132" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="6"/>
-      <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="6"/>
-      <c r="H132" s="6"/>
-      <c r="I132" s="6"/>
-      <c r="J132" s="6"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="7"/>
+      <c r="G132" s="7"/>
+      <c r="H132" s="7"/>
+      <c r="I132" s="7"/>
+      <c r="J132" s="7"/>
     </row>
     <row r="133" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="5" t="s">
@@ -3530,39 +3533,39 @@
       </c>
     </row>
     <row r="134" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
-      <c r="F134" s="7"/>
-      <c r="G134" s="7"/>
-      <c r="H134" s="7"/>
-      <c r="I134" s="7"/>
-      <c r="J134" s="6"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+      <c r="J134" s="7"/>
     </row>
     <row r="135" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="7"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7"/>
-      <c r="E135" s="7"/>
-      <c r="F135" s="7"/>
-      <c r="G135" s="7"/>
-      <c r="H135" s="7"/>
-      <c r="I135" s="7"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="6"/>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
       <c r="J135" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="136" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="6"/>
-      <c r="C136" s="6"/>
-      <c r="D136" s="6"/>
-      <c r="E136" s="6"/>
-      <c r="F136" s="6"/>
-      <c r="G136" s="6"/>
-      <c r="H136" s="6"/>
-      <c r="I136" s="6"/>
-      <c r="J136" s="6"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="7"/>
+      <c r="G136" s="7"/>
+      <c r="H136" s="7"/>
+      <c r="I136" s="7"/>
+      <c r="J136" s="7"/>
     </row>
     <row r="137" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="5" t="s">
@@ -3594,39 +3597,39 @@
       </c>
     </row>
     <row r="138" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
-      <c r="D138" s="7"/>
-      <c r="E138" s="7"/>
-      <c r="F138" s="7"/>
-      <c r="G138" s="7"/>
-      <c r="H138" s="7"/>
-      <c r="I138" s="7"/>
-      <c r="J138" s="6"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+      <c r="F138" s="6"/>
+      <c r="G138" s="6"/>
+      <c r="H138" s="6"/>
+      <c r="I138" s="6"/>
+      <c r="J138" s="7"/>
     </row>
     <row r="139" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-      <c r="G139" s="7"/>
-      <c r="H139" s="7"/>
-      <c r="I139" s="7"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="6"/>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6"/>
       <c r="J139" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="140" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="6"/>
-      <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
-      <c r="F140" s="6"/>
-      <c r="G140" s="6"/>
-      <c r="H140" s="6"/>
-      <c r="I140" s="6"/>
-      <c r="J140" s="6"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+      <c r="F140" s="7"/>
+      <c r="G140" s="7"/>
+      <c r="H140" s="7"/>
+      <c r="I140" s="7"/>
+      <c r="J140" s="7"/>
     </row>
     <row r="141" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B141" s="5" t="s">
@@ -3658,39 +3661,39 @@
       </c>
     </row>
     <row r="142" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-      <c r="G142" s="7"/>
-      <c r="H142" s="7"/>
-      <c r="I142" s="7"/>
-      <c r="J142" s="6"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+      <c r="I142" s="6"/>
+      <c r="J142" s="7"/>
     </row>
     <row r="143" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-      <c r="G143" s="7"/>
-      <c r="H143" s="7"/>
-      <c r="I143" s="7"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
       <c r="J143" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="144" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="6"/>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
-      <c r="H144" s="6"/>
-      <c r="I144" s="6"/>
-      <c r="J144" s="6"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="7"/>
+      <c r="G144" s="7"/>
+      <c r="H144" s="7"/>
+      <c r="I144" s="7"/>
+      <c r="J144" s="7"/>
     </row>
     <row r="145" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="5" t="s">
@@ -3722,39 +3725,39 @@
       </c>
     </row>
     <row r="146" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7"/>
-      <c r="G146" s="7"/>
-      <c r="H146" s="7"/>
-      <c r="I146" s="7"/>
-      <c r="J146" s="6"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
+      <c r="G146" s="6"/>
+      <c r="H146" s="6"/>
+      <c r="I146" s="6"/>
+      <c r="J146" s="7"/>
     </row>
     <row r="147" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
-      <c r="H147" s="7"/>
-      <c r="I147" s="7"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
       <c r="J147" s="5" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="148" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="6"/>
-      <c r="C148" s="6"/>
-      <c r="D148" s="6"/>
-      <c r="E148" s="6"/>
-      <c r="F148" s="6"/>
-      <c r="G148" s="6"/>
-      <c r="H148" s="6"/>
-      <c r="I148" s="6"/>
-      <c r="J148" s="6"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="7"/>
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="7"/>
+      <c r="G148" s="7"/>
+      <c r="H148" s="7"/>
+      <c r="I148" s="7"/>
+      <c r="J148" s="7"/>
     </row>
     <row r="149" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="5" t="s">
@@ -3786,39 +3789,39 @@
       </c>
     </row>
     <row r="150" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="7"/>
-      <c r="H150" s="7"/>
-      <c r="I150" s="7"/>
-      <c r="J150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
+      <c r="H150" s="6"/>
+      <c r="I150" s="6"/>
+      <c r="J150" s="7"/>
     </row>
     <row r="151" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-      <c r="H151" s="7"/>
-      <c r="I151" s="7"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="6"/>
       <c r="J151" s="5" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="152" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="6"/>
-      <c r="C152" s="6"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="6"/>
-      <c r="F152" s="6"/>
-      <c r="G152" s="6"/>
-      <c r="H152" s="6"/>
-      <c r="I152" s="6"/>
-      <c r="J152" s="6"/>
+      <c r="B152" s="7"/>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="7"/>
+      <c r="G152" s="7"/>
+      <c r="H152" s="7"/>
+      <c r="I152" s="7"/>
+      <c r="J152" s="7"/>
     </row>
     <row r="153" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="5" t="s">
@@ -3840,7 +3843,7 @@
         <v>257</v>
       </c>
       <c r="H153" s="8" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="I153" s="9" t="s">
         <v>258</v>
@@ -3850,39 +3853,39 @@
       </c>
     </row>
     <row r="154" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-      <c r="H154" s="7"/>
-      <c r="I154" s="7"/>
-      <c r="J154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6"/>
+      <c r="H154" s="6"/>
+      <c r="I154" s="6"/>
+      <c r="J154" s="7"/>
     </row>
     <row r="155" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-      <c r="H155" s="7"/>
-      <c r="I155" s="7"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6"/>
+      <c r="H155" s="6"/>
+      <c r="I155" s="6"/>
       <c r="J155" s="5" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="156" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="6"/>
-      <c r="C156" s="6"/>
-      <c r="D156" s="6"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
-      <c r="G156" s="6"/>
-      <c r="H156" s="6"/>
-      <c r="I156" s="6"/>
-      <c r="J156" s="6"/>
+      <c r="B156" s="7"/>
+      <c r="C156" s="7"/>
+      <c r="D156" s="7"/>
+      <c r="E156" s="7"/>
+      <c r="F156" s="7"/>
+      <c r="G156" s="7"/>
+      <c r="H156" s="7"/>
+      <c r="I156" s="7"/>
+      <c r="J156" s="7"/>
     </row>
     <row r="157" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="5" t="s">
@@ -3904,7 +3907,7 @@
         <v>257</v>
       </c>
       <c r="H157" s="8" t="s">
-        <v>14</v>
+        <v>268</v>
       </c>
       <c r="I157" s="9" t="s">
         <v>265</v>
@@ -3914,39 +3917,39 @@
       </c>
     </row>
     <row r="158" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-      <c r="F158" s="7"/>
-      <c r="G158" s="7"/>
-      <c r="H158" s="7"/>
-      <c r="I158" s="7"/>
-      <c r="J158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="7"/>
     </row>
     <row r="159" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
-      <c r="H159" s="7"/>
-      <c r="I159" s="7"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
       <c r="J159" s="5" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="160" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="6"/>
-      <c r="C160" s="6"/>
-      <c r="D160" s="6"/>
-      <c r="E160" s="6"/>
-      <c r="F160" s="6"/>
-      <c r="G160" s="6"/>
-      <c r="H160" s="6"/>
-      <c r="I160" s="6"/>
-      <c r="J160" s="6"/>
+      <c r="B160" s="7"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
+      <c r="G160" s="7"/>
+      <c r="H160" s="7"/>
+      <c r="I160" s="7"/>
+      <c r="J160" s="7"/>
     </row>
     <row r="161" spans="5:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E161" s="3"/>
@@ -4255,27 +4258,300 @@
     </row>
   </sheetData>
   <mergeCells count="366">
-    <mergeCell ref="F157:F160"/>
-    <mergeCell ref="E125:E128"/>
-    <mergeCell ref="G157:G160"/>
-    <mergeCell ref="J147:J148"/>
-    <mergeCell ref="F129:F132"/>
-    <mergeCell ref="H129:H132"/>
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J149:J150"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="C153:C156"/>
-    <mergeCell ref="J121:J122"/>
-    <mergeCell ref="J115:J116"/>
-    <mergeCell ref="C125:C128"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="E81:E84"/>
-    <mergeCell ref="G81:G84"/>
-    <mergeCell ref="I81:I84"/>
-    <mergeCell ref="E129:E132"/>
+    <mergeCell ref="J143:J144"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="H77:H80"/>
+    <mergeCell ref="B133:B136"/>
+    <mergeCell ref="D133:D136"/>
+    <mergeCell ref="H97:H100"/>
+    <mergeCell ref="C85:C88"/>
+    <mergeCell ref="J127:J128"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="H69:H72"/>
+    <mergeCell ref="G97:G100"/>
+    <mergeCell ref="I97:I100"/>
+    <mergeCell ref="J103:J104"/>
+    <mergeCell ref="D125:D128"/>
+    <mergeCell ref="F125:F128"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="H81:H84"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="E113:E116"/>
+    <mergeCell ref="J123:J124"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="E121:E124"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="C101:C104"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I45:I48"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="I37:I40"/>
+    <mergeCell ref="J99:J100"/>
+    <mergeCell ref="F113:F116"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="J95:J96"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="E149:E152"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="I117:I120"/>
+    <mergeCell ref="D121:D124"/>
+    <mergeCell ref="F121:F124"/>
+    <mergeCell ref="B141:B144"/>
+    <mergeCell ref="F53:F56"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="E73:E76"/>
+    <mergeCell ref="E137:E140"/>
+    <mergeCell ref="G137:G140"/>
+    <mergeCell ref="C133:C136"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="E101:E104"/>
+    <mergeCell ref="B129:B132"/>
+    <mergeCell ref="D129:D132"/>
+    <mergeCell ref="I41:I44"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="D85:D88"/>
+    <mergeCell ref="H93:H96"/>
+    <mergeCell ref="B149:B152"/>
+    <mergeCell ref="D149:D152"/>
+    <mergeCell ref="H53:H56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="H145:H148"/>
+    <mergeCell ref="G113:G116"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="J137:J138"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J109:J110"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="D73:D76"/>
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D97:D100"/>
+    <mergeCell ref="B121:B124"/>
+    <mergeCell ref="J83:J84"/>
+    <mergeCell ref="G33:G36"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="H65:H68"/>
+    <mergeCell ref="G93:G96"/>
+    <mergeCell ref="G85:G88"/>
+    <mergeCell ref="J117:J118"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="H117:H120"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="I69:I72"/>
+    <mergeCell ref="H37:H40"/>
+    <mergeCell ref="F73:F76"/>
+    <mergeCell ref="I133:I136"/>
+    <mergeCell ref="F137:F140"/>
+    <mergeCell ref="H137:H140"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="J91:J92"/>
+    <mergeCell ref="G37:G40"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="D101:D104"/>
+    <mergeCell ref="F101:F104"/>
+    <mergeCell ref="J133:J134"/>
+    <mergeCell ref="C129:C132"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="J61:J62"/>
+    <mergeCell ref="I153:I156"/>
+    <mergeCell ref="E109:E112"/>
+    <mergeCell ref="J159:J160"/>
+    <mergeCell ref="G109:G112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="D113:D116"/>
+    <mergeCell ref="I65:I68"/>
+    <mergeCell ref="C157:C160"/>
+    <mergeCell ref="I129:I132"/>
+    <mergeCell ref="F89:F92"/>
+    <mergeCell ref="H89:H92"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="H153:H156"/>
+    <mergeCell ref="J145:J146"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="C149:C152"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="E97:E100"/>
+    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="J153:J154"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="G77:G80"/>
+    <mergeCell ref="I77:I80"/>
+    <mergeCell ref="D81:D84"/>
+    <mergeCell ref="G141:G144"/>
+    <mergeCell ref="B145:B148"/>
+    <mergeCell ref="I141:I144"/>
+    <mergeCell ref="D145:D148"/>
+    <mergeCell ref="F145:F148"/>
+    <mergeCell ref="F153:F156"/>
+    <mergeCell ref="F77:F80"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="C81:C84"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="J105:J106"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="I157:I160"/>
+    <mergeCell ref="G149:G152"/>
+    <mergeCell ref="I149:I152"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="H141:H144"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="H41:H44"/>
+    <mergeCell ref="E145:E148"/>
+    <mergeCell ref="C145:C148"/>
+    <mergeCell ref="E117:E120"/>
+    <mergeCell ref="G117:G120"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="I93:I96"/>
+    <mergeCell ref="F97:F100"/>
+    <mergeCell ref="F109:F112"/>
+    <mergeCell ref="I109:I112"/>
+    <mergeCell ref="G41:G44"/>
+    <mergeCell ref="D117:D120"/>
+    <mergeCell ref="F117:F120"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="E157:E160"/>
+    <mergeCell ref="D89:D92"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="J155:J156"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C97:C100"/>
+    <mergeCell ref="G61:G64"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="J157:J158"/>
+    <mergeCell ref="G101:G104"/>
+    <mergeCell ref="I101:I104"/>
+    <mergeCell ref="G125:G128"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="F85:F88"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="H85:H88"/>
+    <mergeCell ref="H109:H112"/>
+    <mergeCell ref="J119:J120"/>
+    <mergeCell ref="D93:D96"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="F93:F96"/>
+    <mergeCell ref="F149:F152"/>
+    <mergeCell ref="H149:H152"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="B137:B140"/>
+    <mergeCell ref="D137:D140"/>
+    <mergeCell ref="D41:D44"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="H101:H104"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="H125:H128"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="G121:G124"/>
+    <mergeCell ref="F41:F44"/>
+    <mergeCell ref="C89:C92"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="G69:G72"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B89:B92"/>
+    <mergeCell ref="B153:B156"/>
+    <mergeCell ref="D69:D72"/>
+    <mergeCell ref="F69:F72"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="F133:F136"/>
+    <mergeCell ref="H133:H136"/>
+    <mergeCell ref="C137:C140"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="J125:J126"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="G65:G68"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="G129:G132"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="J129:J130"/>
+    <mergeCell ref="J107:J108"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="I125:I128"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="C141:C144"/>
+    <mergeCell ref="B109:B112"/>
+    <mergeCell ref="D109:D112"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="J131:J132"/>
+    <mergeCell ref="D153:D156"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="F65:F68"/>
+    <mergeCell ref="H121:H124"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="E141:E144"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="H73:H76"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="J63:J64"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="F81:F84"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="C69:C72"/>
     <mergeCell ref="D157:D160"/>
     <mergeCell ref="G145:G148"/>
     <mergeCell ref="I145:I148"/>
@@ -4300,327 +4576,54 @@
     <mergeCell ref="J39:J40"/>
     <mergeCell ref="E33:E36"/>
     <mergeCell ref="E93:E96"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="C141:C144"/>
-    <mergeCell ref="B109:B112"/>
-    <mergeCell ref="D109:D112"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="J131:J132"/>
-    <mergeCell ref="D153:D156"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="F65:F68"/>
-    <mergeCell ref="H121:H124"/>
-    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="C153:C156"/>
+    <mergeCell ref="J121:J122"/>
+    <mergeCell ref="J115:J116"/>
+    <mergeCell ref="C125:C128"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="E81:E84"/>
+    <mergeCell ref="G81:G84"/>
+    <mergeCell ref="I81:I84"/>
+    <mergeCell ref="E129:E132"/>
     <mergeCell ref="E13:E16"/>
-    <mergeCell ref="E141:E144"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="H73:H76"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="J63:J64"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="F81:F84"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="G49:G52"/>
     <mergeCell ref="G29:G32"/>
     <mergeCell ref="I29:I32"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="C69:C72"/>
     <mergeCell ref="J141:J142"/>
     <mergeCell ref="E85:E88"/>
     <mergeCell ref="J135:J136"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="F25:F28"/>
-    <mergeCell ref="H25:H28"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="F133:F136"/>
-    <mergeCell ref="H133:H136"/>
-    <mergeCell ref="C137:C140"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="J125:J126"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="G65:G68"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="G129:G132"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="J129:J130"/>
-    <mergeCell ref="J107:J108"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="I125:I128"/>
     <mergeCell ref="E133:E136"/>
     <mergeCell ref="G133:G136"/>
-    <mergeCell ref="B137:B140"/>
-    <mergeCell ref="D137:D140"/>
-    <mergeCell ref="D41:D44"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="H101:H104"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="H125:H128"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="G57:G60"/>
     <mergeCell ref="I57:I60"/>
     <mergeCell ref="J79:J80"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="G121:G124"/>
     <mergeCell ref="I121:I124"/>
-    <mergeCell ref="F41:F44"/>
     <mergeCell ref="I11:I12"/>
+    <mergeCell ref="F157:F160"/>
+    <mergeCell ref="E125:E128"/>
+    <mergeCell ref="G157:G160"/>
+    <mergeCell ref="J147:J148"/>
+    <mergeCell ref="F129:F132"/>
+    <mergeCell ref="H129:H132"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J149:J150"/>
     <mergeCell ref="I49:I52"/>
     <mergeCell ref="I113:I116"/>
-    <mergeCell ref="C89:C92"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="G69:G72"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="C17:C20"/>
     <mergeCell ref="H13:H16"/>
     <mergeCell ref="F105:F108"/>
     <mergeCell ref="E77:E80"/>
     <mergeCell ref="H105:H108"/>
     <mergeCell ref="G25:G28"/>
-    <mergeCell ref="D89:D92"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="J155:J156"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="C97:C100"/>
-    <mergeCell ref="G61:G64"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="J157:J158"/>
-    <mergeCell ref="G101:G104"/>
-    <mergeCell ref="I101:I104"/>
-    <mergeCell ref="G125:G128"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="F85:F88"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="H85:H88"/>
-    <mergeCell ref="H109:H112"/>
-    <mergeCell ref="J119:J120"/>
-    <mergeCell ref="D93:D96"/>
-    <mergeCell ref="H57:H60"/>
-    <mergeCell ref="F93:F96"/>
-    <mergeCell ref="F149:F152"/>
-    <mergeCell ref="H149:H152"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="I157:I160"/>
-    <mergeCell ref="G149:G152"/>
-    <mergeCell ref="I149:I152"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="H141:H144"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="H41:H44"/>
-    <mergeCell ref="E145:E148"/>
-    <mergeCell ref="C145:C148"/>
-    <mergeCell ref="E117:E120"/>
-    <mergeCell ref="G117:G120"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="I93:I96"/>
-    <mergeCell ref="F97:F100"/>
-    <mergeCell ref="F109:F112"/>
-    <mergeCell ref="I109:I112"/>
-    <mergeCell ref="G41:G44"/>
-    <mergeCell ref="D117:D120"/>
-    <mergeCell ref="F117:F120"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="E157:E160"/>
     <mergeCell ref="E153:E156"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="C149:C152"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="E97:E100"/>
-    <mergeCell ref="B125:B128"/>
-    <mergeCell ref="J153:J154"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="G17:G20"/>
-    <mergeCell ref="G77:G80"/>
-    <mergeCell ref="I77:I80"/>
-    <mergeCell ref="D81:D84"/>
-    <mergeCell ref="G141:G144"/>
-    <mergeCell ref="B145:B148"/>
-    <mergeCell ref="I141:I144"/>
-    <mergeCell ref="D145:D148"/>
-    <mergeCell ref="F145:F148"/>
-    <mergeCell ref="F153:F156"/>
-    <mergeCell ref="F77:F80"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="C81:C84"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="G45:G48"/>
-    <mergeCell ref="J105:J106"/>
-    <mergeCell ref="J43:J44"/>
     <mergeCell ref="H157:H160"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="J91:J92"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="D101:D104"/>
-    <mergeCell ref="F101:F104"/>
-    <mergeCell ref="J133:J134"/>
-    <mergeCell ref="C129:C132"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="J61:J62"/>
-    <mergeCell ref="I153:I156"/>
-    <mergeCell ref="E109:E112"/>
-    <mergeCell ref="J159:J160"/>
-    <mergeCell ref="G109:G112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="D113:D116"/>
-    <mergeCell ref="I65:I68"/>
-    <mergeCell ref="C157:C160"/>
-    <mergeCell ref="I129:I132"/>
-    <mergeCell ref="F89:F92"/>
-    <mergeCell ref="H89:H92"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="H153:H156"/>
-    <mergeCell ref="J145:J146"/>
     <mergeCell ref="E89:E92"/>
     <mergeCell ref="J139:J140"/>
     <mergeCell ref="G89:G92"/>
     <mergeCell ref="J111:J112"/>
     <mergeCell ref="G153:G156"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="I69:I72"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="F73:F76"/>
-    <mergeCell ref="I133:I136"/>
-    <mergeCell ref="F137:F140"/>
-    <mergeCell ref="H137:H140"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="H65:H68"/>
-    <mergeCell ref="G93:G96"/>
-    <mergeCell ref="G85:G88"/>
-    <mergeCell ref="J117:J118"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="H117:H120"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="J137:J138"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="J109:J110"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="D73:D76"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="D97:D100"/>
-    <mergeCell ref="B121:B124"/>
-    <mergeCell ref="J83:J84"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="G21:G24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="F49:F52"/>
-    <mergeCell ref="D85:D88"/>
-    <mergeCell ref="H93:H96"/>
-    <mergeCell ref="B149:B152"/>
-    <mergeCell ref="D149:D152"/>
-    <mergeCell ref="H53:H56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="E149:E152"/>
-    <mergeCell ref="F33:F36"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="I117:I120"/>
-    <mergeCell ref="D121:D124"/>
-    <mergeCell ref="F121:F124"/>
-    <mergeCell ref="B141:B144"/>
-    <mergeCell ref="F53:F56"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="E73:E76"/>
-    <mergeCell ref="E137:E140"/>
-    <mergeCell ref="G137:G140"/>
-    <mergeCell ref="C133:C136"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="E101:E104"/>
-    <mergeCell ref="B129:B132"/>
-    <mergeCell ref="D129:D132"/>
-    <mergeCell ref="I41:I44"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="H145:H148"/>
-    <mergeCell ref="G113:G116"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="E121:E124"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="C101:C104"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="J74:J75"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I45:I48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="I37:I40"/>
-    <mergeCell ref="J99:J100"/>
-    <mergeCell ref="F113:F116"/>
-    <mergeCell ref="J143:J144"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="H77:H80"/>
-    <mergeCell ref="B133:B136"/>
-    <mergeCell ref="D133:D136"/>
-    <mergeCell ref="H97:H100"/>
-    <mergeCell ref="C85:C88"/>
-    <mergeCell ref="J127:J128"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="D61:D64"/>
-    <mergeCell ref="H69:H72"/>
-    <mergeCell ref="G97:G100"/>
-    <mergeCell ref="I97:I100"/>
-    <mergeCell ref="J103:J104"/>
-    <mergeCell ref="D125:D128"/>
-    <mergeCell ref="F125:F128"/>
-    <mergeCell ref="I17:I20"/>
-    <mergeCell ref="H81:H84"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="E113:E116"/>
-    <mergeCell ref="J123:J124"/>
-    <mergeCell ref="J95:J96"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="J17:J18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E113" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>